<commit_message>
Performed outer join and removed the NaN values.
</commit_message>
<xml_diff>
--- a/movies_merged.xlsx
+++ b/movies_merged.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -852,52 +852,56 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bajirao Mastani </t>
+          <t>The Shawshank Redemption</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bollywood</t>
+          <t>Hollywood</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="E10" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
+        <v>9.300000000000001</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Castle Rock Entertainment</t>
+        </is>
+      </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>1.4</v>
+        <v>25</v>
       </c>
       <c r="I10" t="n">
-        <v>3.5</v>
+        <v>73.3</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Billions</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>USD</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The Shawshank Redemption</t>
+          <t>Interstellar</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -906,24 +910,24 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1994</v>
+        <v>2014</v>
       </c>
       <c r="E11" t="n">
-        <v>9.300000000000001</v>
+        <v>8.6</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Castle Rock Entertainment</t>
+          <t>Warner Bros. Pictures</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>5</v>
       </c>
       <c r="H11" t="n">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="I11" t="n">
-        <v>73.3</v>
+        <v>701.8</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -938,11 +942,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Interstellar</t>
+          <t>The Pursuit of Happyness</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -951,24 +955,24 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="E12" t="n">
-        <v>8.6</v>
+        <v>8</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Warner Bros. Pictures</t>
+          <t>Columbia Pictures</t>
         </is>
       </c>
       <c r="G12" t="n">
         <v>5</v>
       </c>
       <c r="H12" t="n">
-        <v>165</v>
+        <v>55</v>
       </c>
       <c r="I12" t="n">
-        <v>701.8</v>
+        <v>307.1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -983,11 +987,11 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The Pursuit of Happyness</t>
+          <t>Gladiator</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -996,24 +1000,24 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Columbia Pictures</t>
+          <t xml:space="preserve">Universal Pictures  </t>
         </is>
       </c>
       <c r="G13" t="n">
         <v>5</v>
       </c>
       <c r="H13" t="n">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="I13" t="n">
-        <v>307.1</v>
+        <v>460.5</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1028,11 +1032,11 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gladiator</t>
+          <t>Titanic</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1041,24 +1045,24 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="E14" t="n">
-        <v>8.5</v>
+        <v>7.9</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Universal Pictures  </t>
+          <t>Paramount Pictures</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>5</v>
       </c>
       <c r="H14" t="n">
-        <v>103</v>
+        <v>200</v>
       </c>
       <c r="I14" t="n">
-        <v>460.5</v>
+        <v>2202</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1073,11 +1077,11 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Titanic</t>
+          <t>It's a Wonderful Life</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1086,24 +1090,24 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1997</v>
+        <v>1946</v>
       </c>
       <c r="E15" t="n">
-        <v>7.9</v>
+        <v>8.6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Paramount Pictures</t>
+          <t>Liberty Films</t>
         </is>
       </c>
       <c r="G15" t="n">
         <v>5</v>
       </c>
       <c r="H15" t="n">
-        <v>200</v>
+        <v>3.18</v>
       </c>
       <c r="I15" t="n">
-        <v>2202</v>
+        <v>3.3</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1118,11 +1122,11 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>It's a Wonderful Life</t>
+          <t>Avatar</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1131,24 +1135,24 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1946</v>
+        <v>2009</v>
       </c>
       <c r="E16" t="n">
-        <v>8.6</v>
+        <v>7.8</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Liberty Films</t>
+          <t>20th Century Fox</t>
         </is>
       </c>
       <c r="G16" t="n">
         <v>5</v>
       </c>
       <c r="H16" t="n">
-        <v>3.18</v>
+        <v>237</v>
       </c>
       <c r="I16" t="n">
-        <v>3.3</v>
+        <v>2847</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1163,11 +1167,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Avatar</t>
+          <t>The Godfather</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1176,24 +1180,24 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2009</v>
+        <v>1972</v>
       </c>
       <c r="E17" t="n">
-        <v>7.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>20th Century Fox</t>
+          <t>Paramount Pictures</t>
         </is>
       </c>
       <c r="G17" t="n">
         <v>5</v>
       </c>
       <c r="H17" t="n">
-        <v>237</v>
+        <v>7.2</v>
       </c>
       <c r="I17" t="n">
-        <v>2847</v>
+        <v>291</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1208,11 +1212,11 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The Godfather</t>
+          <t>The Dark Knight</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1221,24 +1225,24 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1972</v>
+        <v>2008</v>
       </c>
       <c r="E18" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Paramount Pictures</t>
+          <t>Syncopy</t>
         </is>
       </c>
       <c r="G18" t="n">
         <v>5</v>
       </c>
       <c r="H18" t="n">
-        <v>7.2</v>
+        <v>185</v>
       </c>
       <c r="I18" t="n">
-        <v>291</v>
+        <v>1006</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1253,11 +1257,11 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The Dark Knight</t>
+          <t>Schindler's List</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1266,24 +1270,24 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="E19" t="n">
         <v>9</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Syncopy</t>
+          <t>Universal Pictures</t>
         </is>
       </c>
       <c r="G19" t="n">
         <v>5</v>
       </c>
       <c r="H19" t="n">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="I19" t="n">
-        <v>1006</v>
+        <v>322.2</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1298,11 +1302,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Schindler's List</t>
+          <t>Jurassic Park</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1314,7 +1318,7 @@
         <v>1993</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1325,10 +1329,10 @@
         <v>5</v>
       </c>
       <c r="H20" t="n">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="I20" t="n">
-        <v>322.2</v>
+        <v>1046</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1343,11 +1347,11 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jurassic Park</t>
+          <t>Avengers: Endgame</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1356,24 +1360,24 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1993</v>
+        <v>2019</v>
       </c>
       <c r="E21" t="n">
-        <v>8.199999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Universal Pictures</t>
+          <t>Marvel Studios</t>
         </is>
       </c>
       <c r="G21" t="n">
         <v>5</v>
       </c>
       <c r="H21" t="n">
-        <v>63</v>
+        <v>400</v>
       </c>
       <c r="I21" t="n">
-        <v>1046</v>
+        <v>2798</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1388,11 +1392,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Parasite</t>
+          <t>Avengers: Infinity War</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1401,20 +1405,24 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E22" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+        <v>8.4</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Marvel Studios</t>
+        </is>
+      </c>
       <c r="G22" t="n">
         <v>5</v>
       </c>
       <c r="H22" t="n">
-        <v>15.5</v>
+        <v>400</v>
       </c>
       <c r="I22" t="n">
-        <v>263.1</v>
+        <v>2048</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1429,82 +1437,82 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Avengers: Endgame</t>
+          <t>Pather Panchali</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Hollywood</t>
+          <t>Bollywood</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2019</v>
+        <v>1955</v>
       </c>
       <c r="E23" t="n">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Marvel Studios</t>
+          <t>Government of West Bengal</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H23" t="n">
-        <v>400</v>
+        <v>70000</v>
       </c>
       <c r="I23" t="n">
-        <v>2798</v>
+        <v>100000</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Millions</t>
+          <t>Thousands</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>INR</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Avengers: Infinity War</t>
+          <t>Munna Bhai M.B.B.S.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Hollywood</t>
+          <t>Bollywood</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="E24" t="n">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Marvel Studios</t>
+          <t>Vinod Chopra Productions</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>2048</v>
+        <v>410</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1513,17 +1521,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>INR</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pather Panchali</t>
+          <t>PK</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1532,28 +1540,28 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1955</v>
+        <v>2014</v>
       </c>
       <c r="E25" t="n">
-        <v>8.300000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Government of West Bengal</t>
+          <t>Vinod Chopra Films</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>70000</v>
+        <v>850</v>
       </c>
       <c r="I25" t="n">
-        <v>100000</v>
+        <v>8540</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Thousands</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1564,11 +1572,11 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Taare Zameen Par</t>
+          <t>Pushpa: The Rise - Part 1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1577,24 +1585,28 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2007</v>
+        <v>2021</v>
       </c>
       <c r="E26" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
+        <v>7.6</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Mythri Movie Makers</t>
+        </is>
+      </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" t="n">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="I26" t="n">
-        <v>1350</v>
+        <v>3.6</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Millions</t>
+          <t>Billions</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1605,11 +1617,11 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Munna Bhai M.B.B.S.</t>
+          <t>RRR</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1618,28 +1630,28 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2003</v>
+        <v>2022</v>
       </c>
       <c r="E27" t="n">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Vinod Chopra Productions</t>
+          <t>DVV Entertainment</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>100</v>
+        <v>5.5</v>
       </c>
       <c r="I27" t="n">
-        <v>410</v>
+        <v>12</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Millions</t>
+          <t>Billions</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1650,11 +1662,11 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PK</t>
+          <t>Baahubali: The Beginning</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1663,28 +1675,28 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="E28" t="n">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Vinod Chopra Films</t>
+          <t>Arka Media Works</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="n">
-        <v>850</v>
+        <v>1.8</v>
       </c>
       <c r="I28" t="n">
-        <v>8540</v>
+        <v>6.5</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Millions</t>
+          <t>Billions</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -1695,11 +1707,11 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sanju</t>
+          <t>The Kashmir Files</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1708,26 +1720,28 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2018</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
+        <v>2022</v>
+      </c>
+      <c r="E29" t="n">
+        <v>8.300000000000001</v>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Vinod Chopra Films</t>
+          <t>Zee Studios</t>
         </is>
       </c>
       <c r="G29" t="n">
         <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="I29" t="n">
-        <v>5.9</v>
+        <v>3409</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Billions</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -1738,11 +1752,11 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Pushpa: The Rise - Part 1</t>
+          <t>Bajrangi Bhaijaan</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1751,28 +1765,28 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="E30" t="n">
-        <v>7.6</v>
+        <v>8.1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Mythri Movie Makers</t>
+          <t>Salman Khan Films</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>2</v>
+        <v>900</v>
       </c>
       <c r="I30" t="n">
-        <v>3.6</v>
+        <v>11690</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Billions</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -1783,101 +1797,101 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RRR</t>
+          <t>Captain America: The First Avenger</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bollywood</t>
+          <t>Hollywood</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>6.9</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>DVV Entertainment</t>
+          <t>Marvel Studios</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H31" t="n">
-        <v>5.5</v>
+        <v>216.7</v>
       </c>
       <c r="I31" t="n">
-        <v>12</v>
+        <v>370.6</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Billions</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>USD</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Baahubali: The Beginning</t>
+          <t>Captain America: The Winter Soldier</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bollywood</t>
+          <t>Hollywood</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Arka Media Works</t>
+          <t>Marvel Studios</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H32" t="n">
-        <v>1.8</v>
+        <v>177</v>
       </c>
       <c r="I32" t="n">
-        <v>6.5</v>
+        <v>714.4</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Billions</t>
+          <t>Millions</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>USD</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The Kashmir Files</t>
+          <t>Race 3</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1886,28 +1900,28 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="E33" t="n">
-        <v>8.300000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Zee Studios</t>
+          <t>Salman Khan Films</t>
         </is>
       </c>
       <c r="G33" t="n">
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>250</v>
+        <v>1.8</v>
       </c>
       <c r="I33" t="n">
-        <v>3409</v>
+        <v>3.1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Millions</t>
+          <t>Billions</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -1918,11 +1932,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bajrangi Bhaijaan</t>
+          <t>Shershaah</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1931,24 +1945,24 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E34" t="n">
-        <v>8.1</v>
+        <v>8.4</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Salman Khan Films</t>
+          <t>Dharma Productions</t>
         </is>
       </c>
       <c r="G34" t="n">
         <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="I34" t="n">
-        <v>11690</v>
+        <v>950</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1956,186 +1970,6 @@
         </is>
       </c>
       <c r="K34" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>137</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Captain America: The First Avenger</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Hollywood</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>2011</v>
-      </c>
-      <c r="E35" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Marvel Studios</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
-        <v>5</v>
-      </c>
-      <c r="H35" t="n">
-        <v>216.7</v>
-      </c>
-      <c r="I35" t="n">
-        <v>370.6</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Millions</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>138</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Captain America: The Winter Soldier</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Hollywood</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>2014</v>
-      </c>
-      <c r="E36" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Marvel Studios</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
-        <v>5</v>
-      </c>
-      <c r="H36" t="n">
-        <v>177</v>
-      </c>
-      <c r="I36" t="n">
-        <v>714.4</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Millions</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>139</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Race 3</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Bollywood</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>2018</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Salman Khan Films</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="I37" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Billions</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>140</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Shershaah</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Bollywood</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>2021</v>
-      </c>
-      <c r="E38" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Dharma Productions</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="n">
-        <v>500</v>
-      </c>
-      <c r="I38" t="n">
-        <v>950</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Millions</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
         <is>
           <t>INR</t>
         </is>

</xml_diff>